<commit_message>
done var 1 Excel. Paragraph: user's num format, task 1
</commit_message>
<xml_diff>
--- a/Задания по Экселю/Пользовательские числовые форматы/Задание_1.xlsx
+++ b/Задания по Экселю/Пользовательские числовые форматы/Задание_1.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="28590" windowHeight="12600"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="28590" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Вар. 5" sheetId="2" r:id="rId1"/>
+    <sheet name="Вар. 1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="18">
   <si>
     <t>Оборот за квартал</t>
   </si>
@@ -60,15 +61,25 @@
   </si>
   <si>
     <t>При условии X&gt;=400 ↓</t>
+  </si>
+  <si>
+    <t>Вариант 1</t>
+  </si>
+  <si>
+    <t>При условии X&gt;100 ↓</t>
+  </si>
+  <si>
+    <t>При условии X&lt;30 ↓</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;₽&quot;"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000\ &quot;₽&quot;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -177,49 +188,68 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -527,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -548,62 +578,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="H3" s="5" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="H3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" spans="1:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="4" t="s">
+      <c r="G5" s="17"/>
+      <c r="H5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="8" t="s">
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="11" t="s">
         <v>10</v>
       </c>
     </row>
@@ -621,8 +651,8 @@
       <c r="E6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="17"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
         <v>1</v>
@@ -636,22 +666,22 @@
       <c r="L6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="8"/>
+      <c r="M6" s="11"/>
     </row>
     <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="22">
         <v>1000</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="22">
         <v>-250</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="22">
         <v>340</v>
       </c>
-      <c r="E7" s="16" t="str">
+      <c r="E7" s="8" t="str">
         <f>IF((B7+C7+D7&gt;800), "(2,2,2,2,3)","X&gt;800  не выполняется")</f>
         <v>(2,2,2,2,3)</v>
       </c>
@@ -662,13 +692,13 @@
       <c r="H7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="22">
         <v>1110</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="22">
         <v>760</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="22">
         <v>400</v>
       </c>
       <c r="L7" s="3" t="str">
@@ -681,35 +711,35 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="17" t="str">
+      <c r="A8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="9" t="str">
         <f>IF((B7&gt;0), "(1,1,0,4,2)", IF( (B7&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
-      <c r="C8" s="17" t="str">
+      <c r="C8" s="9" t="str">
         <f>IF((C7&gt;0), "(1,1,0,4,2)", IF( (C7&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(2,1,3,6,6)</v>
       </c>
-      <c r="D8" s="17" t="str">
+      <c r="D8" s="9" t="str">
         <f>IF((D7&gt;0), "(1,1,0,4,2)", IF( (D7&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
-      <c r="E8" s="16"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="2"/>
-      <c r="H8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="17" t="str">
+      <c r="H8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="9" t="str">
         <f>IF((I7&gt;0), "(1,1,0,4,2)", IF( (I7&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
-      <c r="J8" s="17" t="str">
+      <c r="J8" s="9" t="str">
         <f>IF((J7&gt;0), "(1,1,0,4,2)", IF( (J7&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
-      <c r="K8" s="17" t="str">
+      <c r="K8" s="9" t="str">
         <f>IF((K7&gt;0), "(1,1,0,4,2)", IF( (K7&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
@@ -717,19 +747,19 @@
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="22">
         <v>500000</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="22">
         <v>100000</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="22">
         <v>230000</v>
       </c>
-      <c r="E9" s="16" t="str">
+      <c r="E9" s="8" t="str">
         <f>IF((B9+C9+D9&gt;800), "(2,2,2,2,3)","X&gt;800  не выполняется")</f>
         <v>(2,2,2,2,3)</v>
       </c>
@@ -740,13 +770,13 @@
       <c r="H9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="22">
         <v>54300</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="22">
         <v>13500</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="22">
         <v>450</v>
       </c>
       <c r="L9" s="3" t="str">
@@ -759,35 +789,35 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="17" t="str">
+      <c r="A10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="9" t="str">
         <f>IF((B9&gt;0), "(1,1,0,4,2)", IF( (B9&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
-      <c r="C10" s="17" t="str">
+      <c r="C10" s="9" t="str">
         <f>IF((C9&gt;0), "(1,1,0,4,2)", IF( (C9&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
-      <c r="D10" s="17" t="str">
+      <c r="D10" s="9" t="str">
         <f>IF((D9&gt;0), "(1,1,0,4,2)", IF( (D9&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
-      <c r="E10" s="16"/>
+      <c r="E10" s="8"/>
       <c r="F10" s="2"/>
-      <c r="H10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="17" t="str">
+      <c r="H10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="9" t="str">
         <f>IF((I9&gt;0), "(1,1,0,4,2)", IF( (I9&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
-      <c r="J10" s="17" t="str">
+      <c r="J10" s="9" t="str">
         <f>IF((J9&gt;0), "(1,1,0,4,2)", IF( (J9&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
-      <c r="K10" s="17" t="str">
+      <c r="K10" s="9" t="str">
         <f>IF((K9&gt;0), "(1,1,0,4,2)", IF( (K9&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
@@ -798,16 +828,16 @@
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="22">
         <v>0</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="22">
         <v>-350</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="22">
         <v>10</v>
       </c>
-      <c r="E11" s="16" t="str">
+      <c r="E11" s="8" t="str">
         <f>IF((B11+C11+D11&gt;800), "(2,2,2,2,3)","X&gt;800  не выполняется")</f>
         <v>X&gt;800  не выполняется</v>
       </c>
@@ -818,13 +848,13 @@
       <c r="H11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="22">
         <v>255</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="22">
         <v>5440</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="22">
         <v>150</v>
       </c>
       <c r="L11" s="3" t="str">
@@ -837,35 +867,35 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="17" t="str">
+      <c r="A12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="9" t="str">
         <f>IF((B11&gt;0), "(1,1,0,4,2)", IF( (B11&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(2,3,3)</v>
       </c>
-      <c r="C12" s="17" t="str">
+      <c r="C12" s="9" t="str">
         <f>IF((C11&gt;0), "(1,1,0,4,2)", IF( (C11&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(2,1,3,6,6)</v>
       </c>
-      <c r="D12" s="17" t="str">
+      <c r="D12" s="9" t="str">
         <f>IF((D11&gt;0), "(1,1,0,4,2)", IF( (D11&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
-      <c r="E12" s="16"/>
+      <c r="E12" s="8"/>
       <c r="F12" s="2"/>
-      <c r="H12" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="17" t="str">
+      <c r="H12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="9" t="str">
         <f>IF((I11&gt;0), "(1,1,0,4,2)", IF( (I11&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
-      <c r="J12" s="17" t="str">
+      <c r="J12" s="9" t="str">
         <f>IF((J11&gt;0), "(1,1,0,4,2)", IF( (J11&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
-      <c r="K12" s="17" t="str">
+      <c r="K12" s="9" t="str">
         <f>IF((K11&gt;0), "(1,1,0,4,2)", IF( (K11&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
@@ -876,16 +906,16 @@
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="22">
         <v>14000</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="22">
         <v>15000</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="22">
         <v>20000</v>
       </c>
-      <c r="E13" s="16" t="str">
+      <c r="E13" s="8" t="str">
         <f>IF((B13+C13+D13&gt;800), "(2,2,2,2,3)","X&gt;800  не выполняется")</f>
         <v>(2,2,2,2,3)</v>
       </c>
@@ -896,13 +926,13 @@
       <c r="H13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="22">
         <v>350</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="22">
         <v>-5000</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="22">
         <v>3337</v>
       </c>
       <c r="L13" s="3" t="str">
@@ -915,35 +945,35 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="32.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="17" t="str">
+      <c r="A14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="9" t="str">
         <f>IF((B13&gt;0), "(1,1,0,4,2)", IF( (B13&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
-      <c r="C14" s="17" t="str">
+      <c r="C14" s="9" t="str">
         <f>IF((C13&gt;0), "(1,1,0,4,2)", IF( (C13&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
-      <c r="D14" s="17" t="str">
+      <c r="D14" s="9" t="str">
         <f>IF((D13&gt;0), "(1,1,0,4,2)", IF( (D13&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
-      <c r="E14" s="15"/>
+      <c r="E14" s="7"/>
       <c r="F14" s="1"/>
-      <c r="H14" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="17" t="str">
+      <c r="H14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="9" t="str">
         <f>IF((I13&gt;0), "(1,1,0,4,2)", IF( (I13&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
-      <c r="J14" s="17" t="str">
+      <c r="J14" s="9" t="str">
         <f>IF((J13&gt;0), "(1,1,0,4,2)", IF( (J13&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(2,1,3,6,6)</v>
       </c>
-      <c r="K14" s="17" t="str">
+      <c r="K14" s="9" t="str">
         <f>IF((K13&gt;0), "(1,1,0,4,2)", IF( (K13&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
@@ -954,16 +984,16 @@
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="22">
         <v>25000</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="22">
         <v>30000</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="22">
         <v>35000</v>
       </c>
-      <c r="E15" s="16" t="str">
+      <c r="E15" s="8" t="str">
         <f>IF((B15+C15+D15&gt;800), "(2,2,2,2,3)","X&gt;800  не выполняется")</f>
         <v>(2,2,2,2,3)</v>
       </c>
@@ -974,13 +1004,13 @@
       <c r="H15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="22">
         <v>23015</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="22">
         <v>35000</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="22">
         <v>5359</v>
       </c>
       <c r="L15" s="3" t="str">
@@ -993,35 +1023,35 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="17" t="str">
+      <c r="A16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="9" t="str">
         <f>IF((B15&gt;0), "(1,1,0,4,2)", IF( (B15&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
-      <c r="C16" s="17" t="str">
+      <c r="C16" s="9" t="str">
         <f>IF((C15&gt;0), "(1,1,0,4,2)", IF( (C15&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
-      <c r="D16" s="17" t="str">
+      <c r="D16" s="9" t="str">
         <f>IF((D15&gt;0), "(1,1,0,4,2)", IF( (D15&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
-      <c r="E16" s="15"/>
+      <c r="E16" s="7"/>
       <c r="F16" s="1"/>
-      <c r="H16" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="17" t="str">
+      <c r="H16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="9" t="str">
         <f>IF((I15&gt;0), "(1,1,0,4,2)", IF( (I15&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
-      <c r="J16" s="17" t="str">
+      <c r="J16" s="9" t="str">
         <f>IF((J15&gt;0), "(1,1,0,4,2)", IF( (J15&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
-      <c r="K16" s="17" t="str">
+      <c r="K16" s="9" t="str">
         <f>IF((K15&gt;0), "(1,1,0,4,2)", IF( (K15&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
         <v>(1,1,0,4,2)</v>
       </c>
@@ -1043,4 +1073,520 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="20000" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="8" max="8" width="25.5" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" customWidth="1"/>
+    <col min="12" max="12" width="23.1640625" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="H3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="11"/>
+    </row>
+    <row r="7" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="23">
+        <v>50</v>
+      </c>
+      <c r="C7" s="23">
+        <v>-250</v>
+      </c>
+      <c r="D7" s="23">
+        <v>1500</v>
+      </c>
+      <c r="E7" s="18" t="str">
+        <f>IF((B7+C7+D7&gt;100), "(2,2,1,4,1)","X&gt;100 не выполняется")</f>
+        <v>(2,2,1,4,1)</v>
+      </c>
+      <c r="F7" s="19" t="str">
+        <f>IF( (B7+C7+D7)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="24">
+        <v>1110</v>
+      </c>
+      <c r="J7" s="24">
+        <v>760</v>
+      </c>
+      <c r="K7" s="24">
+        <v>400</v>
+      </c>
+      <c r="L7" s="21" t="str">
+        <f>IF((I7+J7+K7&lt;30), "(1,1,3,3,6)","X&lt;30 не выполняется")</f>
+        <v>X&lt;30 не выполняется</v>
+      </c>
+      <c r="M7" s="20" t="str">
+        <f>IF( (I7+J7+K7)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="9" t="str">
+        <f>IF((B7&gt;0), "(1,1,0,1,6)", IF( (B7&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="C8" s="9" t="str">
+        <f>IF((C7&gt;0), "(1,1,0,1,6)", IF( (C7&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(2,2,3,5,1)</v>
+      </c>
+      <c r="D8" s="9" t="str">
+        <f>IF((D7&gt;0), "(1,1,0,1,6)", IF( (D7&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="2"/>
+      <c r="H8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="9" t="str">
+        <f>IF((I7&gt;0), "(1,1,0,1,6)", IF( (I7&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="J8" s="9" t="str">
+        <f>IF((J7&gt;0), "(1,1,0,1,6)", IF( (J7&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="K8" s="9" t="str">
+        <f>IF((K7&gt;0), "(1,1,0,1,6)", IF( (K7&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="23">
+        <v>500000</v>
+      </c>
+      <c r="C9" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D9" s="23">
+        <v>230000</v>
+      </c>
+      <c r="E9" s="18" t="str">
+        <f>IF((B9+C9+D9&gt;100), "(2,2,1,4,1)","X&gt;100 не выполняется")</f>
+        <v>(2,2,1,4,1)</v>
+      </c>
+      <c r="F9" s="19" t="str">
+        <f>IF( (B9+C9+D9)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="23">
+        <v>54300</v>
+      </c>
+      <c r="J9" s="23">
+        <v>13500</v>
+      </c>
+      <c r="K9" s="23">
+        <v>450</v>
+      </c>
+      <c r="L9" s="21" t="str">
+        <f>IF((I9+J9+K9&lt;30), "(1,1,3,3,6)","X&lt;30 не выполняется")</f>
+        <v>X&lt;30 не выполняется</v>
+      </c>
+      <c r="M9" s="19" t="str">
+        <f>IF( (I9+J9+K9)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="21.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="9" t="str">
+        <f>IF((B9&gt;0), "(1,1,0,1,6)", IF( (B9&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="C10" s="9" t="str">
+        <f>IF((C9&gt;0), "(1,1,0,1,6)", IF( (C9&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="D10" s="9" t="str">
+        <f>IF((D9&gt;0), "(1,1,0,1,6)", IF( (D9&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="2"/>
+      <c r="H10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="9" t="str">
+        <f>IF((I9&gt;0), "(1,1,0,1,6)", IF( (I9&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="J10" s="9" t="str">
+        <f>IF((J9&gt;0), "(1,1,0,1,6)", IF( (J9&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="K10" s="9" t="str">
+        <f>IF((K9&gt;0), "(1,1,0,1,6)", IF( (K9&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="22">
+        <v>0</v>
+      </c>
+      <c r="C11" s="22">
+        <v>-350</v>
+      </c>
+      <c r="D11" s="22">
+        <v>10</v>
+      </c>
+      <c r="E11" s="18" t="str">
+        <f>IF((B11+C11+D11&gt;100), "(2,2,1,4,1)","X&gt;100 не выполняется")</f>
+        <v>X&gt;100 не выполняется</v>
+      </c>
+      <c r="F11" s="2" t="str">
+        <f>IF( (B11+C11+D11)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Убыток</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="22">
+        <v>255</v>
+      </c>
+      <c r="J11" s="22">
+        <v>5440</v>
+      </c>
+      <c r="K11" s="22">
+        <v>150</v>
+      </c>
+      <c r="L11" s="21" t="str">
+        <f>IF((I11+J11+K11&lt;30), "(1,1,3,3,6)","X&lt;30 не выполняется")</f>
+        <v>X&lt;30 не выполняется</v>
+      </c>
+      <c r="M11" s="2" t="str">
+        <f>IF( (I11+J11+K11)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="21.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="9" t="str">
+        <f>IF((B11&gt;0), "(1,1,0,1,6)", IF( (B11&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(3,2,6)</v>
+      </c>
+      <c r="C12" s="9" t="str">
+        <f>IF((C11&gt;0), "(1,1,0,1,6)", IF( (C11&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(2,2,3,5,1)</v>
+      </c>
+      <c r="D12" s="9" t="str">
+        <f>IF((D11&gt;0), "(1,1,0,1,6)", IF( (D11&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="2"/>
+      <c r="H12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="9" t="str">
+        <f>IF((I11&gt;0), "(1,1,0,1,6)", IF( (I11&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="J12" s="9" t="str">
+        <f>IF((J11&gt;0), "(1,1,0,1,6)", IF( (J11&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="K12" s="9" t="str">
+        <f>IF((K11&gt;0), "(1,1,0,1,6)", IF( (K11&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="23">
+        <v>14000</v>
+      </c>
+      <c r="C13" s="23">
+        <v>15000</v>
+      </c>
+      <c r="D13" s="23">
+        <v>20000</v>
+      </c>
+      <c r="E13" s="18" t="str">
+        <f>IF((B13+C13+D13&gt;100), "(2,2,1,4,1)","X&gt;100 не выполняется")</f>
+        <v>(2,2,1,4,1)</v>
+      </c>
+      <c r="F13" s="19" t="str">
+        <f>IF( (B13+C13+D13)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="22">
+        <v>350</v>
+      </c>
+      <c r="J13" s="22">
+        <v>-5000</v>
+      </c>
+      <c r="K13" s="22">
+        <v>3337</v>
+      </c>
+      <c r="L13" s="21" t="str">
+        <f>IF((I13+J13+K13&lt;30), "(1,1,3,3,6)","X&lt;30 не выполняется")</f>
+        <v>(1,1,3,3,6)</v>
+      </c>
+      <c r="M13" s="2" t="str">
+        <f>IF( (I13+J13+K13)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Убыток</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="21.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="9" t="str">
+        <f>IF((B13&gt;0), "(1,1,0,1,6)", IF( (B13&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="C14" s="9" t="str">
+        <f>IF((C13&gt;0), "(1,1,0,1,6)", IF( (C13&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="D14" s="9" t="str">
+        <f>IF((D13&gt;0), "(1,1,0,1,6)", IF( (D13&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="1"/>
+      <c r="H14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="9" t="str">
+        <f>IF((I13&gt;0), "(1,1,0,1,6)", IF( (I13&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="J14" s="9" t="str">
+        <f>IF((J13&gt;0), "(1,1,0,1,6)", IF( (J13&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(2,2,3,5,1)</v>
+      </c>
+      <c r="K14" s="9" t="str">
+        <f>IF((K13&gt;0), "(1,1,0,1,6)", IF( (K13&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="23">
+        <v>25000</v>
+      </c>
+      <c r="C15" s="23">
+        <v>30000</v>
+      </c>
+      <c r="D15" s="23">
+        <v>35000</v>
+      </c>
+      <c r="E15" s="18" t="str">
+        <f>IF((B15+C15+D15&gt;100), "(2,2,1,4,1)","X&gt;100 не выполняется")</f>
+        <v>(2,2,1,4,1)</v>
+      </c>
+      <c r="F15" s="19" t="str">
+        <f>IF( (B15+C15+D15)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="22">
+        <v>23015</v>
+      </c>
+      <c r="J15" s="22">
+        <v>35000</v>
+      </c>
+      <c r="K15" s="22">
+        <v>5359</v>
+      </c>
+      <c r="L15" s="21" t="str">
+        <f>IF((I15+J15+K15&lt;30), "(1,1,3,3,6)","X&lt;30 не выполняется")</f>
+        <v>X&lt;30 не выполняется</v>
+      </c>
+      <c r="M15" s="2" t="str">
+        <f>IF( (I15+J15+K15)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="21.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="9" t="str">
+        <f>IF((B15&gt;0), "(1,1,0,1,6)", IF( (B15&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="C16" s="9" t="str">
+        <f>IF((C15&gt;0), "(1,1,0,1,6)", IF( (C15&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="D16" s="9" t="str">
+        <f>IF((D15&gt;0), "(1,1,0,1,6)", IF( (D15&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="1"/>
+      <c r="H16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="9" t="str">
+        <f>IF((I15&gt;0), "(1,1,0,1,6)", IF( (I15&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="J16" s="9" t="str">
+        <f>IF((J15&gt;0), "(1,1,0,1,6)", IF( (J15&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="K16" s="9" t="str">
+        <f>IF((K15&gt;0), "(1,1,0,1,6)", IF( (K15&lt;0), "(2,2,3,5,1)", "(3,2,6)"))</f>
+        <v>(1,1,0,1,6)</v>
+      </c>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="M5:M6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
done var 3 Excel. Paragraph: user's num format, task 1
</commit_message>
<xml_diff>
--- a/Задания по Экселю/Пользовательские числовые форматы/Задание_1.xlsx
+++ b/Задания по Экселю/Пользовательские числовые форматы/Задание_1.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="28590" windowHeight="12600" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="28590" windowHeight="12600" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Вар. 1" sheetId="3" r:id="rId1"/>
     <sheet name="Вар. 2" sheetId="4" r:id="rId2"/>
-    <sheet name="Вар. 5" sheetId="2" r:id="rId3"/>
+    <sheet name="Вар. 3" sheetId="5" r:id="rId3"/>
+    <sheet name="Вар. 5" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="24">
   <si>
     <t>Оборот за квартал</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t>При условии X&lt;0 ↓</t>
+  </si>
+  <si>
+    <t>Вариант 3</t>
+  </si>
+  <si>
+    <t>При условии X&gt;1000 ↓</t>
+  </si>
+  <si>
+    <t>При условии X ≠ 300 ↓</t>
   </si>
 </sst>
 </file>
@@ -199,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -247,6 +256,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -271,9 +304,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -282,24 +312,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -624,60 +636,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="H3" s="20" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="H3" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="31"/>
       <c r="F5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="25" t="s">
+      <c r="G5" s="32"/>
+      <c r="H5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="26" t="s">
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="34" t="s">
         <v>10</v>
       </c>
     </row>
@@ -696,7 +708,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="6"/>
-      <c r="G6" s="24"/>
+      <c r="G6" s="32"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
         <v>1</v>
@@ -710,7 +722,7 @@
       <c r="L6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="26"/>
+      <c r="M6" s="34"/>
     </row>
     <row r="7" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -832,7 +844,7 @@
         <v>Прибыль</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="21.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="32.25" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -910,7 +922,7 @@
         <v>Прибыль</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="21.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="32.25" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
@@ -988,7 +1000,7 @@
         <v>Убыток</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="21.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="32.25" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
@@ -1066,7 +1078,7 @@
         <v>Прибыль</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="21.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="32.25" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -1120,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1140,96 +1152,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="H3" s="20" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="H3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="30"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="37"/>
       <c r="F5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="26" t="s">
+      <c r="G5" s="32"/>
+      <c r="H5" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26" t="s">
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27" t="s">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="20" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="17"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27" t="s">
+      <c r="G6" s="32"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="J6" s="27" t="s">
+      <c r="J6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="27" t="s">
+      <c r="K6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="L6" s="27" t="s">
+      <c r="L6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="26"/>
+      <c r="M6" s="34"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="15">
@@ -1241,7 +1253,7 @@
       <c r="D7" s="15">
         <v>1500</v>
       </c>
-      <c r="E7" s="34" t="str">
+      <c r="E7" s="24" t="str">
         <f>IF((B7+C7+D7&gt;500), "(2,1,2,2,4)","X&gt;500 не выполняется")</f>
         <v>(2,1,2,2,4)</v>
       </c>
@@ -1249,8 +1261,8 @@
         <f>IF( (B7+C7+D7)&gt;1000, "Прибыль", "Убыток")</f>
         <v>Прибыль</v>
       </c>
-      <c r="G7" s="31"/>
-      <c r="H7" s="27" t="s">
+      <c r="G7" s="21"/>
+      <c r="H7" s="20" t="s">
         <v>5</v>
       </c>
       <c r="I7" s="16">
@@ -1266,13 +1278,13 @@
         <f>IF((I7+J7+K7&lt;0), "(2,1,2,2,4)","X&lt;0 не выполняется")</f>
         <v>X&lt;0 не выполняется</v>
       </c>
-      <c r="M7" s="36" t="str">
+      <c r="M7" s="26" t="str">
         <f>IF( (I7+J7+K7)&gt;1000, "Прибыль", "Убыток")</f>
         <v>Прибыль</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="21" x14ac:dyDescent="0.2">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="22" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="9" t="str">
@@ -1287,10 +1299,10 @@
         <f>IF((D7&gt;0),"(1,2,1,1,5)",IF((D7&lt;0),"(2,1,2,2,2)","(2,5,4)"))</f>
         <v>(1,2,1,1,5)</v>
       </c>
-      <c r="E8" s="34"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="32" t="s">
+      <c r="G8" s="21"/>
+      <c r="H8" s="22" t="s">
         <v>11</v>
       </c>
       <c r="I8" s="9" t="str">
@@ -1305,11 +1317,11 @@
         <f>IF((K7&gt;0),"(1,2,1,1,5)",IF((K7&lt;0),"(2,1,2,2,2)","(2,5,4)"))</f>
         <v>(1,2,1,1,5)</v>
       </c>
-      <c r="L8" s="35"/>
-      <c r="M8" s="27"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="20"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="23" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="15">
@@ -1321,7 +1333,7 @@
       <c r="D9" s="15">
         <v>230000</v>
       </c>
-      <c r="E9" s="34" t="str">
+      <c r="E9" s="24" t="str">
         <f>IF((B9+C9+D9&gt;500), "(2,1,2,2,4)","X&gt;500 не выполняется")</f>
         <v>(2,1,2,2,4)</v>
       </c>
@@ -1329,8 +1341,8 @@
         <f>IF( (B9+C9+D9)&gt;1000, "Прибыль", "Убыток")</f>
         <v>Прибыль</v>
       </c>
-      <c r="G9" s="31"/>
-      <c r="H9" s="27" t="s">
+      <c r="G9" s="21"/>
+      <c r="H9" s="20" t="s">
         <v>6</v>
       </c>
       <c r="I9" s="15">
@@ -1352,7 +1364,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="21" x14ac:dyDescent="0.2">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="22" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="9" t="str">
@@ -1367,10 +1379,10 @@
         <f>IF((D9&gt;0),"(1,2,1,1,5)",IF((D9&lt;0),"(2,1,2,2,2)","(2,5,4)"))</f>
         <v>(1,2,1,1,5)</v>
       </c>
-      <c r="E10" s="34"/>
+      <c r="E10" s="24"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="32" t="s">
+      <c r="G10" s="21"/>
+      <c r="H10" s="22" t="s">
         <v>11</v>
       </c>
       <c r="I10" s="9" t="str">
@@ -1385,11 +1397,11 @@
         <f>IF((K9&gt;0),"(1,2,1,1,5)",IF((K9&lt;0),"(2,1,2,2,2)","(2,5,4)"))</f>
         <v>(1,2,1,1,5)</v>
       </c>
-      <c r="L10" s="35"/>
-      <c r="M10" s="27"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="20"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="20" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="15">
@@ -1401,7 +1413,7 @@
       <c r="D11" s="15">
         <v>10</v>
       </c>
-      <c r="E11" s="34" t="str">
+      <c r="E11" s="24" t="str">
         <f>IF((B11+C11+D11&gt;500), "(2,1,2,2,4)","X&gt;500 не выполняется")</f>
         <v>X&gt;500 не выполняется</v>
       </c>
@@ -1409,8 +1421,8 @@
         <f>IF( (B11+C11+D11)&gt;1000, "Прибыль", "Убыток")</f>
         <v>Убыток</v>
       </c>
-      <c r="G11" s="31"/>
-      <c r="H11" s="27" t="s">
+      <c r="G11" s="21"/>
+      <c r="H11" s="20" t="s">
         <v>7</v>
       </c>
       <c r="I11" s="15">
@@ -1432,7 +1444,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="21" x14ac:dyDescent="0.2">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="22" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="9" t="str">
@@ -1447,10 +1459,10 @@
         <f>IF((D11&gt;0),"(1,2,1,1,5)",IF((D11&lt;0),"(2,1,2,2,2)","(2,5,4)"))</f>
         <v>(1,2,1,1,5)</v>
       </c>
-      <c r="E12" s="34"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="11"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="32" t="s">
+      <c r="G12" s="21"/>
+      <c r="H12" s="22" t="s">
         <v>11</v>
       </c>
       <c r="I12" s="9" t="str">
@@ -1465,11 +1477,11 @@
         <f>IF((K11&gt;0),"(1,2,1,1,5)",IF((K11&lt;0),"(2,1,2,2,2)","(2,5,4)"))</f>
         <v>(1,2,1,1,5)</v>
       </c>
-      <c r="L12" s="35"/>
-      <c r="M12" s="27"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="20"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="15">
@@ -1481,7 +1493,7 @@
       <c r="D13" s="15">
         <v>20000</v>
       </c>
-      <c r="E13" s="34" t="str">
+      <c r="E13" s="24" t="str">
         <f>IF((B13+C13+D13&gt;500), "(2,1,2,2,4)","X&gt;500 не выполняется")</f>
         <v>(2,1,2,2,4)</v>
       </c>
@@ -1489,8 +1501,8 @@
         <f>IF( (B13+C13+D13)&gt;1000, "Прибыль", "Убыток")</f>
         <v>Прибыль</v>
       </c>
-      <c r="G13" s="31"/>
-      <c r="H13" s="27" t="s">
+      <c r="G13" s="21"/>
+      <c r="H13" s="20" t="s">
         <v>8</v>
       </c>
       <c r="I13" s="15">
@@ -1511,8 +1523,8 @@
         <v>Убыток</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="32" t="s">
+    <row r="14" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="9" t="str">
@@ -1528,9 +1540,9 @@
         <v>(1,2,1,1,5)</v>
       </c>
       <c r="E14" s="9"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="32" t="s">
+      <c r="F14" s="20"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="22" t="s">
         <v>11</v>
       </c>
       <c r="I14" s="9" t="str">
@@ -1545,11 +1557,11 @@
         <f>IF((K13&gt;0),"(1,2,1,1,5)",IF((K13&lt;0),"(2,1,2,2,2)","(2,5,4)"))</f>
         <v>(2,1,2,2,2)</v>
       </c>
-      <c r="L14" s="35"/>
-      <c r="M14" s="27"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="20"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="15">
@@ -1561,7 +1573,7 @@
       <c r="D15" s="15">
         <v>35000</v>
       </c>
-      <c r="E15" s="34" t="str">
+      <c r="E15" s="24" t="str">
         <f>IF((B15+C15+D15&gt;500), "(2,1,2,2,4)","X&gt;500 не выполняется")</f>
         <v>(2,1,2,2,4)</v>
       </c>
@@ -1569,8 +1581,8 @@
         <f>IF( (B15+C15+D15)&gt;1000, "Прибыль", "Убыток")</f>
         <v>Прибыль</v>
       </c>
-      <c r="G15" s="31"/>
-      <c r="H15" s="27" t="s">
+      <c r="G15" s="21"/>
+      <c r="H15" s="20" t="s">
         <v>9</v>
       </c>
       <c r="I15" s="15">
@@ -1592,7 +1604,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="21" x14ac:dyDescent="0.2">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="22" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="9" t="str">
@@ -1608,9 +1620,9 @@
         <v>(1,2,1,1,5)</v>
       </c>
       <c r="E16" s="9"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="32" t="s">
+      <c r="F16" s="20"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="22" t="s">
         <v>11</v>
       </c>
       <c r="I16" s="9" t="str">
@@ -1625,8 +1637,8 @@
         <f>IF((K15&gt;0),"(1,2,1,1,5)",IF((K15&lt;0),"(2,1,2,2,2)","(2,5,4)"))</f>
         <v>(1,2,1,1,5)</v>
       </c>
-      <c r="L16" s="35"/>
-      <c r="M16" s="27"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="20"/>
     </row>
     <row r="17" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L17" s="18"/>
@@ -1646,6 +1658,504 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" customWidth="1"/>
+    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" customWidth="1"/>
+    <col min="10" max="10" width="23.1640625" customWidth="1"/>
+    <col min="11" max="11" width="23" customWidth="1"/>
+    <col min="12" max="12" width="22.1640625" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="H3" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="32"/>
+      <c r="H5" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="34"/>
+    </row>
+    <row r="7" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="15">
+        <v>100</v>
+      </c>
+      <c r="C7" s="15">
+        <v>100</v>
+      </c>
+      <c r="D7" s="15">
+        <v>100</v>
+      </c>
+      <c r="E7" s="24" t="str">
+        <f>IF((B7+C7+D7&lt;&gt;300),"X ≠ 300 
+не выполняется","1,1,3,3,3")</f>
+        <v>1,1,3,3,3</v>
+      </c>
+      <c r="F7" s="11" t="str">
+        <f>IF( (B7+C7+D7)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Убыток</v>
+      </c>
+      <c r="G7" s="21"/>
+      <c r="H7" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="16">
+        <v>1110</v>
+      </c>
+      <c r="J7" s="16">
+        <v>-760</v>
+      </c>
+      <c r="K7" s="16">
+        <v>0</v>
+      </c>
+      <c r="L7" s="24" t="str">
+        <f>IF((I7+J7+K7&gt;1000), "2,1,2,6,2","X&gt;1000 
+не выполняется")</f>
+        <v>X&gt;1000 
+не выполняется</v>
+      </c>
+      <c r="M7" s="26" t="str">
+        <f>IF( (I7+J7+K7)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Убыток</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="9" t="str">
+        <f>IF((I7&gt;0),"2,1,2,2,4",IF((I7&lt;0),"1,1,1,3,3","1,3,4"))</f>
+        <v>2,1,2,2,4</v>
+      </c>
+      <c r="J8" s="9" t="str">
+        <f>IF((J7&gt;0),"2,1,2,2,4",IF((J7&lt;0),"1,1,1,3,3","1,3,4"))</f>
+        <v>1,1,1,3,3</v>
+      </c>
+      <c r="K8" s="9" t="str">
+        <f>IF((K7&gt;0),"2,1,2,2,4",IF((K7&lt;0),"1,1,1,3,3","1,3,4"))</f>
+        <v>1,3,4</v>
+      </c>
+      <c r="L8" s="25"/>
+      <c r="M8" s="20"/>
+    </row>
+    <row r="9" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="15">
+        <v>500000</v>
+      </c>
+      <c r="C9" s="15">
+        <v>100000</v>
+      </c>
+      <c r="D9" s="15">
+        <v>230000</v>
+      </c>
+      <c r="E9" s="24" t="str">
+        <f>IF((B9+C9+D9&lt;&gt;300),"X ≠ 300 
+не выполняется","1,1,3,3,3")</f>
+        <v>X ≠ 300 
+не выполняется</v>
+      </c>
+      <c r="F9" s="11" t="str">
+        <f>IF( (B9+C9+D9)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+      <c r="G9" s="21"/>
+      <c r="H9" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="15">
+        <v>1100</v>
+      </c>
+      <c r="J9" s="15">
+        <v>152</v>
+      </c>
+      <c r="K9" s="15">
+        <v>150</v>
+      </c>
+      <c r="L9" s="24" t="str">
+        <f>IF((I9+J9+K9&gt;1000), "2,1,2,6,2","X&gt;1000 
+не выполняется")</f>
+        <v>2,1,2,6,2</v>
+      </c>
+      <c r="M9" s="11" t="str">
+        <f>IF( (I9+J9+K9)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="9" t="str">
+        <f>IF((I9&gt;0),"2,1,2,2,4",IF((I9&lt;0),"1,1,1,3,3","1,3,4"))</f>
+        <v>2,1,2,2,4</v>
+      </c>
+      <c r="J10" s="9" t="str">
+        <f>IF((J9&gt;0),"2,1,2,2,4",IF((J9&lt;0),"1,1,1,3,3","1,3,4"))</f>
+        <v>2,1,2,2,4</v>
+      </c>
+      <c r="K10" s="9" t="str">
+        <f>IF((K9&gt;0),"2,1,2,2,4",IF((K9&lt;0),"1,1,1,3,3","1,3,4"))</f>
+        <v>2,1,2,2,4</v>
+      </c>
+      <c r="L10" s="25"/>
+      <c r="M10" s="20"/>
+    </row>
+    <row r="11" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="15">
+        <v>0</v>
+      </c>
+      <c r="C11" s="15">
+        <v>-350</v>
+      </c>
+      <c r="D11" s="15">
+        <v>10</v>
+      </c>
+      <c r="E11" s="24" t="str">
+        <f>IF((B11+C11+D11&lt;&gt;300),"X ≠ 300 
+не выполняется","1,1,3,3,3")</f>
+        <v>X ≠ 300 
+не выполняется</v>
+      </c>
+      <c r="F11" s="11" t="str">
+        <f>IF( (B11+C11+D11)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Убыток</v>
+      </c>
+      <c r="G11" s="21"/>
+      <c r="H11" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="15">
+        <v>200</v>
+      </c>
+      <c r="J11" s="15">
+        <v>50</v>
+      </c>
+      <c r="K11" s="15">
+        <v>50</v>
+      </c>
+      <c r="L11" s="24" t="str">
+        <f>IF((I11+J11+K11&gt;1000), "2,1,2,6,2","X&gt;1000 
+не выполняется")</f>
+        <v>X&gt;1000 
+не выполняется</v>
+      </c>
+      <c r="M11" s="11" t="str">
+        <f>IF( (I11+J11+K11)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Убыток</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="9" t="str">
+        <f>IF((I11&gt;0),"2,1,2,2,4",IF((I11&lt;0),"1,1,1,3,3","1,3,4"))</f>
+        <v>2,1,2,2,4</v>
+      </c>
+      <c r="J12" s="9" t="str">
+        <f>IF((J11&gt;0),"2,1,2,2,4",IF((J11&lt;0),"1,1,1,3,3","1,3,4"))</f>
+        <v>2,1,2,2,4</v>
+      </c>
+      <c r="K12" s="9" t="str">
+        <f>IF((K11&gt;0),"2,1,2,2,4",IF((K11&lt;0),"1,1,1,3,3","1,3,4"))</f>
+        <v>2,1,2,2,4</v>
+      </c>
+      <c r="L12" s="25"/>
+      <c r="M12" s="20"/>
+    </row>
+    <row r="13" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="15">
+        <v>14000</v>
+      </c>
+      <c r="C13" s="15">
+        <v>15000</v>
+      </c>
+      <c r="D13" s="15">
+        <v>20000</v>
+      </c>
+      <c r="E13" s="24" t="str">
+        <f>IF((B13+C13+D13&lt;&gt;300),"X ≠ 300 
+не выполняется","1,1,3,3,3")</f>
+        <v>X ≠ 300 
+не выполняется</v>
+      </c>
+      <c r="F13" s="11" t="str">
+        <f>IF( (B13+C13+D13)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+      <c r="G13" s="21"/>
+      <c r="H13" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="15">
+        <v>-350</v>
+      </c>
+      <c r="J13" s="15">
+        <v>-5000</v>
+      </c>
+      <c r="K13" s="15">
+        <v>-3337</v>
+      </c>
+      <c r="L13" s="24" t="str">
+        <f>IF((I13+J13+K13&gt;1000), "2,1,2,6,2","X&gt;1000 
+не выполняется")</f>
+        <v>X&gt;1000 
+не выполняется</v>
+      </c>
+      <c r="M13" s="11" t="str">
+        <f>IF( (I13+J13+K13)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Убыток</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="9" t="str">
+        <f>IF((I13&gt;0),"2,1,2,2,4",IF((I13&lt;0),"1,1,1,3,3","1,3,4"))</f>
+        <v>1,1,1,3,3</v>
+      </c>
+      <c r="J14" s="9" t="str">
+        <f>IF((J13&gt;0),"2,1,2,2,4",IF((J13&lt;0),"1,1,1,3,3","1,3,4"))</f>
+        <v>1,1,1,3,3</v>
+      </c>
+      <c r="K14" s="9" t="str">
+        <f>IF((K13&gt;0),"2,1,2,2,4",IF((K13&lt;0),"1,1,1,3,3","1,3,4"))</f>
+        <v>1,1,1,3,3</v>
+      </c>
+      <c r="L14" s="25"/>
+      <c r="M14" s="20"/>
+    </row>
+    <row r="15" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="15">
+        <v>25000</v>
+      </c>
+      <c r="C15" s="15">
+        <v>30000</v>
+      </c>
+      <c r="D15" s="15">
+        <v>35000</v>
+      </c>
+      <c r="E15" s="24" t="str">
+        <f>IF((B15+C15+D15&lt;&gt;300),"X ≠ 300 
+не выполняется","1,1,3,3,3")</f>
+        <v>X ≠ 300 
+не выполняется</v>
+      </c>
+      <c r="F15" s="11" t="str">
+        <f>IF( (B15+C15+D15)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+      <c r="G15" s="21"/>
+      <c r="H15" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="15">
+        <v>23015</v>
+      </c>
+      <c r="J15" s="15">
+        <v>35000</v>
+      </c>
+      <c r="K15" s="15">
+        <v>5359</v>
+      </c>
+      <c r="L15" s="24" t="str">
+        <f>IF((I15+J15+K15&gt;1000), "2,1,2,6,2","X&gt;1000 не выполняется")</f>
+        <v>2,1,2,6,2</v>
+      </c>
+      <c r="M15" s="11" t="str">
+        <f>IF( (I15+J15+K15)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+      <c r="A16" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="9" t="str">
+        <f>IF((I15&gt;0),"2,1,2,2,4",IF((I15&lt;0),"1,1,1,3,3","1,3,4"))</f>
+        <v>2,1,2,2,4</v>
+      </c>
+      <c r="J16" s="9" t="str">
+        <f>IF((J15&gt;0),"2,1,2,2,4",IF((J15&lt;0),"1,1,1,3,3","1,3,4"))</f>
+        <v>2,1,2,2,4</v>
+      </c>
+      <c r="K16" s="9" t="str">
+        <f>IF((K15&gt;0),"2,1,2,2,4",IF((K15&lt;0),"1,1,1,3,3","1,3,4"))</f>
+        <v>2,1,2,2,4</v>
+      </c>
+      <c r="L16" s="25"/>
+      <c r="M16" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="M5:M6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
@@ -1670,62 +2180,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
     </row>
     <row r="2" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="H3" s="20" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="H3" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
     </row>
     <row r="4" spans="1:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="31"/>
       <c r="F5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="25" t="s">
+      <c r="G5" s="32"/>
+      <c r="H5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="26" t="s">
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="34" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1744,7 +2254,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="6"/>
-      <c r="G6" s="24"/>
+      <c r="G6" s="32"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
         <v>1</v>
@@ -1758,7 +2268,7 @@
       <c r="L6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="26"/>
+      <c r="M6" s="34"/>
     </row>
     <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">

</xml_diff>

<commit_message>
done var 4 Excel. Paragraph: user's num format, task 1
</commit_message>
<xml_diff>
--- a/Задания по Экселю/Пользовательские числовые форматы/Задание_1.xlsx
+++ b/Задания по Экселю/Пользовательские числовые форматы/Задание_1.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="28590" windowHeight="12600" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="28590" windowHeight="12600" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Вар. 1" sheetId="3" r:id="rId1"/>
     <sheet name="Вар. 2" sheetId="4" r:id="rId2"/>
     <sheet name="Вар. 3" sheetId="5" r:id="rId3"/>
-    <sheet name="Вар. 5" sheetId="2" r:id="rId4"/>
+    <sheet name="Вар. 4" sheetId="6" r:id="rId4"/>
+    <sheet name="Вар. 5" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="27">
   <si>
     <t>Оборот за квартал</t>
   </si>
@@ -90,6 +91,15 @@
   </si>
   <si>
     <t>При условии X ≠ 300 ↓</t>
+  </si>
+  <si>
+    <t>Вариант 4</t>
+  </si>
+  <si>
+    <t>При условии X == 700 ↓</t>
+  </si>
+  <si>
+    <t>При условии X&lt;200 ↓</t>
   </si>
 </sst>
 </file>
@@ -208,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -279,6 +289,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -636,60 +649,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="H3" s="28" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="H3" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="31"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="32"/>
       <c r="F5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="32"/>
-      <c r="H5" s="33" t="s">
+      <c r="G5" s="33"/>
+      <c r="H5" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="34" t="s">
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="35" t="s">
         <v>10</v>
       </c>
     </row>
@@ -708,7 +721,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="6"/>
-      <c r="G6" s="32"/>
+      <c r="G6" s="33"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
         <v>1</v>
@@ -722,7 +735,7 @@
       <c r="L6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="34"/>
+      <c r="M6" s="35"/>
     </row>
     <row r="7" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -1152,60 +1165,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="H3" s="28" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="H3" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="37"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="38"/>
       <c r="F5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="32"/>
-      <c r="H5" s="34" t="s">
+      <c r="G5" s="33"/>
+      <c r="H5" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34" t="s">
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1224,7 +1237,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="17"/>
-      <c r="G6" s="32"/>
+      <c r="G6" s="33"/>
       <c r="H6" s="20"/>
       <c r="I6" s="20" t="s">
         <v>1</v>
@@ -1238,7 +1251,7 @@
       <c r="L6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="34"/>
+      <c r="M6" s="35"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
@@ -1661,8 +1674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1682,60 +1695,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="H3" s="28" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="H3" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="37"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="38"/>
       <c r="F5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="32"/>
-      <c r="H5" s="34" t="s">
+      <c r="G5" s="33"/>
+      <c r="H5" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34" t="s">
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1754,7 +1767,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="19"/>
-      <c r="G6" s="32"/>
+      <c r="G6" s="33"/>
       <c r="H6" s="20"/>
       <c r="I6" s="20" t="s">
         <v>1</v>
@@ -1768,7 +1781,7 @@
       <c r="L6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="34"/>
+      <c r="M6" s="35"/>
     </row>
     <row r="7" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
@@ -2157,10 +2170,543 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="22.83203125" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="12.5" customWidth="1"/>
+    <col min="12" max="12" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="H3" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="33"/>
+      <c r="H5" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="27"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="35"/>
+    </row>
+    <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="15">
+        <v>500</v>
+      </c>
+      <c r="C7" s="15">
+        <v>100</v>
+      </c>
+      <c r="D7" s="15">
+        <v>100</v>
+      </c>
+      <c r="E7" s="24" t="str">
+        <f>IF((B7+C7+D7=700),"1,2,0,4,5","X не равен 700")</f>
+        <v>1,2,0,4,5</v>
+      </c>
+      <c r="F7" s="11" t="str">
+        <f>IF( (B7+C7+D7)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Убыток</v>
+      </c>
+      <c r="G7" s="21"/>
+      <c r="H7" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="16">
+        <v>110</v>
+      </c>
+      <c r="J7" s="16">
+        <v>-760</v>
+      </c>
+      <c r="K7" s="16">
+        <v>0</v>
+      </c>
+      <c r="L7" s="24" t="str">
+        <f>IF((I7+J7+K7&lt;200), "2,2,3,6,3","X&lt;200 
+не выполняется")</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="M7" s="26" t="str">
+        <f>IF( (I7+J7+K7)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Убыток</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="52.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="9" t="str">
+        <f>IF((B7&gt;0), "2,2,3,6,3", IF( (B7&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="C8" s="9" t="str">
+        <f>IF((C7&gt;0), "2,2,3,6,3", IF( (C7&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="D8" s="9" t="str">
+        <f>IF((D7&gt;0), "2,2,3,6,3", IF( (D7&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="E8" s="24"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="9" t="str">
+        <f>IF((I7&gt;0), "2,2,3,6,3", IF( (I7&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="J8" s="9" t="str">
+        <f>IF((J7&gt;0), "2,2,3,6,3", IF( (J7&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>1,2,0,4,5</v>
+      </c>
+      <c r="K8" s="9" t="str">
+        <f>IF((K7&gt;0), "2,2,3,6,3", IF( (K7&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>3,4,2</v>
+      </c>
+      <c r="L8" s="25"/>
+      <c r="M8" s="20"/>
+    </row>
+    <row r="9" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="15">
+        <v>500000</v>
+      </c>
+      <c r="C9" s="15">
+        <v>100000</v>
+      </c>
+      <c r="D9" s="15">
+        <v>230000</v>
+      </c>
+      <c r="E9" s="24" t="str">
+        <f>IF((B9+C9+D9=700),"1,2,0,4,5","X не равен 700")</f>
+        <v>X не равен 700</v>
+      </c>
+      <c r="F9" s="11" t="str">
+        <f>IF( (B9+C9+D9)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+      <c r="G9" s="21"/>
+      <c r="H9" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="15">
+        <v>1100</v>
+      </c>
+      <c r="J9" s="15">
+        <v>152</v>
+      </c>
+      <c r="K9" s="15">
+        <v>150</v>
+      </c>
+      <c r="L9" s="24" t="str">
+        <f>IF((I9+J9+K9&lt;200), "2,2,3,6,3","X&lt;200 
+не выполняется")</f>
+        <v>X&lt;200 
+не выполняется</v>
+      </c>
+      <c r="M9" s="11" t="str">
+        <f>IF( (I9+J9+K9)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="52.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="9" t="str">
+        <f>IF((B9&gt;0), "2,2,3,6,3", IF( (B9&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="C10" s="9" t="str">
+        <f>IF((C9&gt;0), "2,2,3,6,3", IF( (C9&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="D10" s="9" t="str">
+        <f>IF((D9&gt;0), "2,2,3,6,3", IF( (D9&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="E10" s="24"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="9" t="str">
+        <f>IF((I9&gt;0), "2,2,3,6,3", IF( (I9&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="J10" s="9" t="str">
+        <f>IF((J9&gt;0), "2,2,3,6,3", IF( (J9&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="K10" s="9" t="str">
+        <f>IF((K9&gt;0), "2,2,3,6,3", IF( (K9&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="L10" s="25"/>
+      <c r="M10" s="20"/>
+    </row>
+    <row r="11" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="15">
+        <v>0</v>
+      </c>
+      <c r="C11" s="15">
+        <v>-350</v>
+      </c>
+      <c r="D11" s="15">
+        <v>10</v>
+      </c>
+      <c r="E11" s="24" t="str">
+        <f>IF((B11+C11+D11=700),"1,2,0,4,5","X не равен 700")</f>
+        <v>X не равен 700</v>
+      </c>
+      <c r="F11" s="11" t="str">
+        <f>IF( (B11+C11+D11)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Убыток</v>
+      </c>
+      <c r="G11" s="21"/>
+      <c r="H11" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="15">
+        <v>200</v>
+      </c>
+      <c r="J11" s="15">
+        <v>50</v>
+      </c>
+      <c r="K11" s="15">
+        <v>50</v>
+      </c>
+      <c r="L11" s="24" t="str">
+        <f>IF((I11+J11+K11&lt;200), "2,2,3,6,3","X&lt;200 
+не выполняется")</f>
+        <v>X&lt;200 
+не выполняется</v>
+      </c>
+      <c r="M11" s="11" t="str">
+        <f>IF( (I11+J11+K11)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Убыток</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="52.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="9" t="str">
+        <f>IF((B11&gt;0), "2,2,3,6,3", IF( (B11&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>3,4,2</v>
+      </c>
+      <c r="C12" s="9" t="str">
+        <f>IF((C11&gt;0), "2,2,3,6,3", IF( (C11&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>1,2,0,4,5</v>
+      </c>
+      <c r="D12" s="9" t="str">
+        <f>IF((D11&gt;0), "2,2,3,6,3", IF( (D11&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="E12" s="24"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="9" t="str">
+        <f>IF((I11&gt;0), "2,2,3,6,3", IF( (I11&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="J12" s="9" t="str">
+        <f>IF((J11&gt;0), "2,2,3,6,3", IF( (J11&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="K12" s="9" t="str">
+        <f>IF((K11&gt;0), "2,2,3,6,3", IF( (K11&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="L12" s="25"/>
+      <c r="M12" s="20"/>
+    </row>
+    <row r="13" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="15">
+        <v>14000</v>
+      </c>
+      <c r="C13" s="15">
+        <v>15000</v>
+      </c>
+      <c r="D13" s="15">
+        <v>20000</v>
+      </c>
+      <c r="E13" s="24" t="str">
+        <f>IF((B13+C13+D13=700),"1,2,0,4,5","X не равен 700")</f>
+        <v>X не равен 700</v>
+      </c>
+      <c r="F13" s="11" t="str">
+        <f>IF( (B13+C13+D13)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+      <c r="G13" s="21"/>
+      <c r="H13" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="15">
+        <v>-350</v>
+      </c>
+      <c r="J13" s="15">
+        <v>-5000</v>
+      </c>
+      <c r="K13" s="15">
+        <v>-3337</v>
+      </c>
+      <c r="L13" s="24" t="str">
+        <f>IF((I13+J13+K13&lt;200), "2,2,3,6,3","X&lt;200 
+не выполняется")</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="M13" s="11" t="str">
+        <f>IF( (I13+J13+K13)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Убыток</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="52.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="9" t="str">
+        <f>IF((B13&gt;0), "2,2,3,6,3", IF( (B13&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="C14" s="9" t="str">
+        <f>IF((C13&gt;0), "2,2,3,6,3", IF( (C13&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="D14" s="9" t="str">
+        <f>IF((D13&gt;0), "2,2,3,6,3", IF( (D13&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="9" t="str">
+        <f>IF((I13&gt;0), "2,2,3,6,3", IF( (I13&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>1,2,0,4,5</v>
+      </c>
+      <c r="J14" s="9" t="str">
+        <f>IF((J13&gt;0), "2,2,3,6,3", IF( (J13&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>1,2,0,4,5</v>
+      </c>
+      <c r="K14" s="9" t="str">
+        <f>IF((K13&gt;0), "2,2,3,6,3", IF( (K13&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>1,2,0,4,5</v>
+      </c>
+      <c r="L14" s="25"/>
+      <c r="M14" s="20"/>
+    </row>
+    <row r="15" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="15">
+        <v>25000</v>
+      </c>
+      <c r="C15" s="15">
+        <v>30000</v>
+      </c>
+      <c r="D15" s="15">
+        <v>35000</v>
+      </c>
+      <c r="E15" s="24" t="str">
+        <f>IF((B15+C15+D15=700),"1,2,0,4,5","X не равен 700")</f>
+        <v>X не равен 700</v>
+      </c>
+      <c r="F15" s="11" t="str">
+        <f>IF( (B15+C15+D15)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+      <c r="G15" s="21"/>
+      <c r="H15" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="15">
+        <v>23015</v>
+      </c>
+      <c r="J15" s="15">
+        <v>35000</v>
+      </c>
+      <c r="K15" s="15">
+        <v>5359</v>
+      </c>
+      <c r="L15" s="24" t="str">
+        <f>IF((I15+J15+K15&lt;200), "2,2,3,6,3","X&lt;200 
+не выполняется")</f>
+        <v>X&lt;200 
+не выполняется</v>
+      </c>
+      <c r="M15" s="11" t="str">
+        <f>IF( (I15+J15+K15)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="52.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="9" t="str">
+        <f>IF((B15&gt;0), "2,2,3,6,3", IF( (B15&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="C16" s="9" t="str">
+        <f>IF((C15&gt;0), "2,2,3,6,3", IF( (C15&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="D16" s="9" t="str">
+        <f>IF((D15&gt;0), "2,2,3,6,3", IF( (D15&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="9" t="str">
+        <f>IF((I15&gt;0), "2,2,3,6,3", IF( (I15&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="J16" s="9" t="str">
+        <f>IF((J15&gt;0), "2,2,3,6,3", IF( (J15&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="K16" s="9" t="str">
+        <f>IF((K15&gt;0), "2,2,3,6,3", IF( (K15&lt;0), "1,2,0,4,5", "3,4,2"))</f>
+        <v>2,2,3,6,3</v>
+      </c>
+      <c r="L16" s="25"/>
+      <c r="M16" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="M5:M6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2180,62 +2726,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
     </row>
     <row r="2" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="H3" s="28" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="H3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
     </row>
     <row r="4" spans="1:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="31"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="32"/>
       <c r="F5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="32"/>
-      <c r="H5" s="33" t="s">
+      <c r="G5" s="33"/>
+      <c r="H5" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="34" t="s">
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="35" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2254,7 +2800,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="6"/>
-      <c r="G6" s="32"/>
+      <c r="G6" s="33"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
         <v>1</v>
@@ -2268,7 +2814,7 @@
       <c r="L6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="34"/>
+      <c r="M6" s="35"/>
     </row>
     <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">

</xml_diff>

<commit_message>
done var 6 Excel. Paragraph: user's num format, task 1
</commit_message>
<xml_diff>
--- a/Задания по Экселю/Пользовательские числовые форматы/Задание_1.xlsx
+++ b/Задания по Экселю/Пользовательские числовые форматы/Задание_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="28590" windowHeight="12600" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="28590" windowHeight="12600" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Вар. 1" sheetId="3" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Вар. 3" sheetId="5" r:id="rId3"/>
     <sheet name="Вар. 4" sheetId="6" r:id="rId4"/>
     <sheet name="Вар. 5" sheetId="2" r:id="rId5"/>
+    <sheet name="Вар. 6" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="29">
   <si>
     <t>Оборот за квартал</t>
   </si>
@@ -60,19 +61,7 @@
     <t>Вариант 5</t>
   </si>
   <si>
-    <t>При условии X&gt;800 ↓</t>
-  </si>
-  <si>
-    <t>При условии X&gt;=400 ↓</t>
-  </si>
-  <si>
     <t>Вариант 1</t>
-  </si>
-  <si>
-    <t>При условии X&gt;100 ↓</t>
-  </si>
-  <si>
-    <t>При условии X&lt;30 ↓</t>
   </si>
   <si>
     <t>Вариант 2</t>
@@ -87,19 +76,37 @@
     <t>Вариант 3</t>
   </si>
   <si>
-    <t>При условии X&gt;1000 ↓</t>
-  </si>
-  <si>
-    <t>При условии X ≠ 300 ↓</t>
-  </si>
-  <si>
     <t>Вариант 4</t>
   </si>
   <si>
-    <t>При условии X == 700 ↓</t>
+    <t>Вариант 6</t>
   </si>
   <si>
-    <t>При условии X&lt;200 ↓</t>
+    <t>При условии, что Итого: X ≠ 300 ↓</t>
+  </si>
+  <si>
+    <t>При условии, что Итого: X&gt;1000 ↓</t>
+  </si>
+  <si>
+    <t>При условии, что Итого: X&gt;100 ↓</t>
+  </si>
+  <si>
+    <t>При условии, что Итого: X&lt;30 ↓</t>
+  </si>
+  <si>
+    <t>При условии, что Итого: X == 700 ↓</t>
+  </si>
+  <si>
+    <t>При условии, что Итого: X&lt;200 ↓</t>
+  </si>
+  <si>
+    <t>При условии, что Итого: X&gt;800 ↓</t>
+  </si>
+  <si>
+    <t>При условии, что Итого: X&gt;=400 ↓</t>
+  </si>
+  <si>
+    <t>При условии, что Итого: X ≠ 100 ↓</t>
   </si>
 </sst>
 </file>
@@ -218,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -289,6 +296,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -630,7 +640,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M16" sqref="A1:M16"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -649,60 +659,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
+      <c r="A1" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="H3" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
+      <c r="A3" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="H3" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="33"/>
       <c r="F5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="33"/>
-      <c r="H5" s="34" t="s">
+      <c r="G5" s="34"/>
+      <c r="H5" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="35" t="s">
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="36" t="s">
         <v>10</v>
       </c>
     </row>
@@ -721,7 +731,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="6"/>
-      <c r="G6" s="33"/>
+      <c r="G6" s="34"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
         <v>1</v>
@@ -735,7 +745,7 @@
       <c r="L6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="35"/>
+      <c r="M6" s="36"/>
     </row>
     <row r="7" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -1165,60 +1175,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
+      <c r="A1" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="H3" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
+      <c r="A3" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="H3" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="38"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="39"/>
       <c r="F5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="33"/>
-      <c r="H5" s="35" t="s">
+      <c r="G5" s="34"/>
+      <c r="H5" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35" t="s">
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1237,7 +1247,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="17"/>
-      <c r="G6" s="33"/>
+      <c r="G6" s="34"/>
       <c r="H6" s="20"/>
       <c r="I6" s="20" t="s">
         <v>1</v>
@@ -1251,7 +1261,7 @@
       <c r="L6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="35"/>
+      <c r="M6" s="36"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
@@ -1675,7 +1685,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="A3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1695,60 +1705,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="H3" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="H3" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="38"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="39"/>
       <c r="F5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="33"/>
-      <c r="H5" s="35" t="s">
+      <c r="G5" s="34"/>
+      <c r="H5" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35" t="s">
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1767,7 +1777,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="19"/>
-      <c r="G6" s="33"/>
+      <c r="G6" s="34"/>
       <c r="H6" s="20"/>
       <c r="I6" s="20" t="s">
         <v>1</v>
@@ -1781,7 +1791,7 @@
       <c r="L6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="35"/>
+      <c r="M6" s="36"/>
     </row>
     <row r="7" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
@@ -2172,8 +2182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2191,60 +2201,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="H3" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="H3" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="38"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="39"/>
       <c r="F5" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="33"/>
-      <c r="H5" s="35" t="s">
+      <c r="G5" s="34"/>
+      <c r="H5" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35" t="s">
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2263,7 +2273,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="27"/>
-      <c r="G6" s="33"/>
+      <c r="G6" s="34"/>
       <c r="H6" s="20"/>
       <c r="I6" s="20" t="s">
         <v>1</v>
@@ -2277,9 +2287,9 @@
       <c r="L6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="35"/>
-    </row>
-    <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.2">
+      <c r="M6" s="36"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
         <v>5</v>
       </c>
@@ -2323,7 +2333,7 @@
         <v>Убыток</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="52.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="21" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>11</v>
       </c>
@@ -2405,7 +2415,7 @@
         <v>Прибыль</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="52.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="21" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
         <v>11</v>
       </c>
@@ -2487,7 +2497,7 @@
         <v>Убыток</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="52.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="21" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
         <v>11</v>
       </c>
@@ -2568,7 +2578,7 @@
         <v>Убыток</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="52.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="21" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
         <v>11</v>
       </c>
@@ -2650,7 +2660,7 @@
         <v>Прибыль</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="52.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="21" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
         <v>11</v>
       </c>
@@ -2705,8 +2715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2726,62 +2736,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
     </row>
     <row r="2" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="H3" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
+      <c r="A3" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="H3" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
     </row>
     <row r="4" spans="1:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="33"/>
       <c r="F5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="33"/>
-      <c r="H5" s="34" t="s">
+      <c r="G5" s="34"/>
+      <c r="H5" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="35" t="s">
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="36" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2800,7 +2810,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="6"/>
-      <c r="G6" s="33"/>
+      <c r="G6" s="34"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
         <v>1</v>
@@ -2814,7 +2824,7 @@
       <c r="L6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="35"/>
+      <c r="M6" s="36"/>
     </row>
     <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -3221,4 +3231,518 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="20000" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="10" max="11" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="23.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="H3" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="28"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="36"/>
+    </row>
+    <row r="7" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="14">
+        <v>0</v>
+      </c>
+      <c r="C7" s="14">
+        <v>0</v>
+      </c>
+      <c r="D7" s="14">
+        <v>100</v>
+      </c>
+      <c r="E7" s="8" t="str">
+        <f>IF((B7+C7+D7&lt;&gt;100), "1,1,0,4,2", "Условие X ≠ 100 не выполняется")</f>
+        <v>Условие X ≠ 100 не выполняется</v>
+      </c>
+      <c r="F7" s="2" t="str">
+        <f>IF( (B7+C7+D7)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Убыток</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="14">
+        <v>1110</v>
+      </c>
+      <c r="J7" s="14">
+        <v>760</v>
+      </c>
+      <c r="K7" s="14">
+        <v>400</v>
+      </c>
+      <c r="L7" s="3" t="str">
+        <f>IF((I7+J7+K7&gt;1000), "(2,1,3,6,6)","X&gt;1000  не выполняется")</f>
+        <v>(2,1,3,6,6)</v>
+      </c>
+      <c r="M7" s="2" t="str">
+        <f>IF( (I7+J7+K7)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="53.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="9" t="str">
+        <f>IF((B7&gt;0), "(1,1,0,4,2)", IF( (B7&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(2,3,3)</v>
+      </c>
+      <c r="C8" s="9" t="str">
+        <f>IF((C7&gt;0), "(1,1,0,4,2)", IF( (C7&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(2,3,3)</v>
+      </c>
+      <c r="D8" s="9" t="str">
+        <f>IF((D7&gt;0), "(1,1,0,4,2)", IF( (D7&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="2"/>
+      <c r="H8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="9" t="str">
+        <f>IF((I7&gt;0), "(1,1,0,4,2)", IF( (I7&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="J8" s="9" t="str">
+        <f>IF((J7&gt;0), "(1,1,0,4,2)", IF( (J7&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="K8" s="9" t="str">
+        <f>IF((K7&gt;0), "(1,1,0,4,2)", IF( (K7&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="14">
+        <v>500000</v>
+      </c>
+      <c r="C9" s="14">
+        <v>100000</v>
+      </c>
+      <c r="D9" s="14">
+        <v>230000</v>
+      </c>
+      <c r="E9" s="8" t="str">
+        <f>IF((B9+C9+D9&lt;&gt;100), "1,1,0,4,2", "Условие X ≠ 100 не выполняется")</f>
+        <v>1,1,0,4,2</v>
+      </c>
+      <c r="F9" s="2" t="str">
+        <f>IF( (B9+C9+D9)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="14">
+        <v>54300</v>
+      </c>
+      <c r="J9" s="14">
+        <v>13500</v>
+      </c>
+      <c r="K9" s="14">
+        <v>450</v>
+      </c>
+      <c r="L9" s="3" t="str">
+        <f>IF((I9+J9+K9&gt;1000), "(2,1,3,6,6)","X&gt;1000  не выполняется")</f>
+        <v>(2,1,3,6,6)</v>
+      </c>
+      <c r="M9" s="2" t="str">
+        <f>IF( (I9+J9+K9)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="53.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="9" t="str">
+        <f>IF((B9&gt;0), "(1,1,0,4,2)", IF( (B9&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="C10" s="9" t="str">
+        <f>IF((C9&gt;0), "(1,1,0,4,2)", IF( (C9&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="D10" s="9" t="str">
+        <f>IF((D9&gt;0), "(1,1,0,4,2)", IF( (D9&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="2"/>
+      <c r="H10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="9" t="str">
+        <f>IF((I9&gt;0), "(1,1,0,4,2)", IF( (I9&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="J10" s="9" t="str">
+        <f>IF((J9&gt;0), "(1,1,0,4,2)", IF( (J9&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="K10" s="9" t="str">
+        <f>IF((K9&gt;0), "(1,1,0,4,2)", IF( (K9&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="14">
+        <v>0</v>
+      </c>
+      <c r="C11" s="14">
+        <v>-350</v>
+      </c>
+      <c r="D11" s="14">
+        <v>10</v>
+      </c>
+      <c r="E11" s="8" t="str">
+        <f>IF((B11+C11+D11&lt;&gt;100), "1,1,0,4,2", "Условие X ≠ 100 не выполняется")</f>
+        <v>1,1,0,4,2</v>
+      </c>
+      <c r="F11" s="2" t="str">
+        <f>IF( (B11+C11+D11)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Убыток</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="14">
+        <v>255</v>
+      </c>
+      <c r="J11" s="14">
+        <v>5440</v>
+      </c>
+      <c r="K11" s="14">
+        <v>150</v>
+      </c>
+      <c r="L11" s="3" t="str">
+        <f>IF((I11+J11+K11&gt;1000), "(2,1,3,6,6)","X&gt;1000  не выполняется")</f>
+        <v>(2,1,3,6,6)</v>
+      </c>
+      <c r="M11" s="2" t="str">
+        <f>IF( (I11+J11+K11)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="53.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="9" t="str">
+        <f>IF((B11&gt;0), "(1,1,0,4,2)", IF( (B11&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(2,3,3)</v>
+      </c>
+      <c r="C12" s="9" t="str">
+        <f>IF((C11&gt;0), "(1,1,0,4,2)", IF( (C11&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(2,1,3,6,6)</v>
+      </c>
+      <c r="D12" s="9" t="str">
+        <f>IF((D11&gt;0), "(1,1,0,4,2)", IF( (D11&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="2"/>
+      <c r="H12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="9" t="str">
+        <f>IF((I11&gt;0), "(1,1,0,4,2)", IF( (I11&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="J12" s="9" t="str">
+        <f>IF((J11&gt;0), "(1,1,0,4,2)", IF( (J11&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="K12" s="9" t="str">
+        <f>IF((K11&gt;0), "(1,1,0,4,2)", IF( (K11&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="14">
+        <v>14000</v>
+      </c>
+      <c r="C13" s="14">
+        <v>15000</v>
+      </c>
+      <c r="D13" s="14">
+        <v>20000</v>
+      </c>
+      <c r="E13" s="8" t="str">
+        <f>IF((B13+C13+D13&lt;&gt;100), "1,1,0,4,2", "Условие X ≠ 100 не выполняется")</f>
+        <v>1,1,0,4,2</v>
+      </c>
+      <c r="F13" s="2" t="str">
+        <f>IF( (B13+C13+D13)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="14">
+        <v>350</v>
+      </c>
+      <c r="J13" s="14">
+        <v>-5000</v>
+      </c>
+      <c r="K13" s="14">
+        <v>3337</v>
+      </c>
+      <c r="L13" s="3" t="str">
+        <f>IF((I13+J13+K13&gt;1000), "(2,1,3,6,6)","X&gt;1000  не выполняется")</f>
+        <v>X&gt;1000  не выполняется</v>
+      </c>
+      <c r="M13" s="2" t="str">
+        <f>IF( (I13+J13+K13)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Убыток</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="53.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="9" t="str">
+        <f>IF((B13&gt;0), "(1,1,0,4,2)", IF( (B13&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="C14" s="9" t="str">
+        <f>IF((C13&gt;0), "(1,1,0,4,2)", IF( (C13&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="D14" s="9" t="str">
+        <f>IF((D13&gt;0), "(1,1,0,4,2)", IF( (D13&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="1"/>
+      <c r="H14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="9" t="str">
+        <f>IF((I13&gt;0), "(1,1,0,4,2)", IF( (I13&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="J14" s="9" t="str">
+        <f>IF((J13&gt;0), "(1,1,0,4,2)", IF( (J13&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(2,1,3,6,6)</v>
+      </c>
+      <c r="K14" s="9" t="str">
+        <f>IF((K13&gt;0), "(1,1,0,4,2)", IF( (K13&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="14">
+        <v>25000</v>
+      </c>
+      <c r="C15" s="14">
+        <v>30000</v>
+      </c>
+      <c r="D15" s="14">
+        <v>35000</v>
+      </c>
+      <c r="E15" s="8" t="str">
+        <f>IF((B15+C15+D15&lt;&gt;100), "1,1,0,4,2", "Условие X ≠ 100 не выполняется")</f>
+        <v>1,1,0,4,2</v>
+      </c>
+      <c r="F15" s="2" t="str">
+        <f>IF( (B15+C15+D15)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="14">
+        <v>23015</v>
+      </c>
+      <c r="J15" s="14">
+        <v>35000</v>
+      </c>
+      <c r="K15" s="14">
+        <v>5359</v>
+      </c>
+      <c r="L15" s="3" t="str">
+        <f>IF((I15+J15+K15&gt;1000), "(2,1,3,6,6)","X&gt;1000  не выполняется")</f>
+        <v>(2,1,3,6,6)</v>
+      </c>
+      <c r="M15" s="2" t="str">
+        <f>IF( (I15+J15+K15)&gt;1000, "Прибыль", "Убыток")</f>
+        <v>Прибыль</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="53.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="9" t="str">
+        <f>IF((B15&gt;0), "(1,1,0,4,2)", IF( (B15&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="C16" s="9" t="str">
+        <f>IF((C15&gt;0), "(1,1,0,4,2)", IF( (C15&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="D16" s="9" t="str">
+        <f>IF((D15&gt;0), "(1,1,0,4,2)", IF( (D15&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="1"/>
+      <c r="H16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="9" t="str">
+        <f>IF((I15&gt;0), "(1,1,0,4,2)", IF( (I15&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="J16" s="9" t="str">
+        <f>IF((J15&gt;0), "(1,1,0,4,2)", IF( (J15&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="K16" s="9" t="str">
+        <f>IF((K15&gt;0), "(1,1,0,4,2)", IF( (K15&lt;0), "(2,1,3,6,6)", "(2,3,3)"))</f>
+        <v>(1,1,0,4,2)</v>
+      </c>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="M5:M6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>